<commit_message>
updates on the ReadMe.md
</commit_message>
<xml_diff>
--- a/mc4c_DatasetStatistics.xlsx
+++ b/mc4c_DatasetStatistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aallahyar/Technical/My_Works/MC-4C/67_MC4C_In_Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADF7753-01F9-6448-BBEB-ED9A9A594F05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA352549-79AE-C94F-A6BC-75A6668DCAF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="1740" windowWidth="28800" windowHeight="17540" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="195">
   <si>
     <t>MinION</t>
   </si>
@@ -598,6 +598,18 @@
   </si>
   <si>
     <t>532ng</t>
+  </si>
+  <si>
+    <t>asMC4C_mESC_WT_A</t>
+  </si>
+  <si>
+    <t>deLaat_asMC4C_mESC_WT_A</t>
+  </si>
+  <si>
+    <t>FAK27205</t>
+  </si>
+  <si>
+    <t>313ng</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A1970-D648-A84B-9973-6E2CBBFEC5E9}">
-  <dimension ref="A1:AH42"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3067,6 +3079,29 @@
         <v>190</v>
       </c>
     </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B43" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="18">
+        <v>43516</v>
+      </c>
+      <c r="J43" t="s">
+        <v>193</v>
+      </c>
+      <c r="K43">
+        <v>1710</v>
+      </c>
+      <c r="Q43" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new config files
</commit_message>
<xml_diff>
--- a/mc4c_DatasetStatistics.xlsx
+++ b/mc4c_DatasetStatistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aallahyar/Technical/My_Works/MC-4C/67_MC4C_In_Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF06C5E-85C8-D942-A4F0-655A8807059D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D997BF-9EA3-4A48-BFC6-1A2E6C789EC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="1740" windowWidth="28800" windowHeight="17540" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="207">
   <si>
     <t>MinION</t>
   </si>
@@ -637,6 +637,15 @@
   </si>
   <si>
     <t>83ng</t>
+  </si>
+  <si>
+    <t>asMC4C_INV_C</t>
+  </si>
+  <si>
+    <t>FAK57663</t>
+  </si>
+  <si>
+    <t>74ng</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A1970-D648-A84B-9973-6E2CBBFEC5E9}">
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AH47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3198,6 +3207,29 @@
         <v>203</v>
       </c>
     </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="18">
+        <v>43558</v>
+      </c>
+      <c r="J47" t="s">
+        <v>205</v>
+      </c>
+      <c r="K47">
+        <v>1375</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new stats for latest MC-4C runs
</commit_message>
<xml_diff>
--- a/mc4c_DatasetStatistics.xlsx
+++ b/mc4c_DatasetStatistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aallahyar/Technical/My_Works/MC-4C/67_MC4C_In_Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D997BF-9EA3-4A48-BFC6-1A2E6C789EC2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656491B7-74B7-FF4C-9B81-4B80160C0218}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="1740" windowWidth="28800" windowHeight="17540" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
   <si>
     <t>MinION</t>
   </si>
@@ -646,6 +651,24 @@
   </si>
   <si>
     <t>74ng</t>
+  </si>
+  <si>
+    <t>asMC4C_INV_A</t>
+  </si>
+  <si>
+    <t>GridION spike more library after 50 min</t>
+  </si>
+  <si>
+    <t>FAK56942</t>
+  </si>
+  <si>
+    <t>70ng</t>
+  </si>
+  <si>
+    <t>asMC4C_WT_C_II</t>
+  </si>
+  <si>
+    <t>FAK57299</t>
   </si>
 </sst>
 </file>
@@ -1073,21 +1096,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A1970-D648-A84B-9973-6E2CBBFEC5E9}">
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AH49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
@@ -3230,6 +3253,58 @@
         <v>206</v>
       </c>
     </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" t="s">
+        <v>208</v>
+      </c>
+      <c r="G48" s="18">
+        <v>43573</v>
+      </c>
+      <c r="J48" t="s">
+        <v>209</v>
+      </c>
+      <c r="K48">
+        <v>1424</v>
+      </c>
+      <c r="P48" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>211</v>
+      </c>
+      <c r="B49" t="s">
+        <v>211</v>
+      </c>
+      <c r="E49" t="s">
+        <v>208</v>
+      </c>
+      <c r="G49" s="18">
+        <v>43573</v>
+      </c>
+      <c r="J49" t="s">
+        <v>212</v>
+      </c>
+      <c r="K49">
+        <v>1415</v>
+      </c>
+      <c r="P49" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added pore stats for RB_WT
</commit_message>
<xml_diff>
--- a/mc4c_DatasetStatistics.xlsx
+++ b/mc4c_DatasetStatistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aallahyar/Technical/My_Works/MC-4C/67_MC4C_In_Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656491B7-74B7-FF4C-9B81-4B80160C0218}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB876645-4986-944B-BE11-81F4553C8DE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="1740" windowWidth="28800" windowHeight="17540" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
   </bookViews>
   <sheets>
     <sheet name="SeqMachine_stats" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="218">
   <si>
     <t>MinION</t>
   </si>
@@ -669,6 +669,21 @@
   </si>
   <si>
     <t>FAK57299</t>
+  </si>
+  <si>
+    <t>VER3768</t>
+  </si>
+  <si>
+    <t>nano cis</t>
+  </si>
+  <si>
+    <t>refuel</t>
+  </si>
+  <si>
+    <t>FAK83014</t>
+  </si>
+  <si>
+    <t>596ng</t>
   </si>
 </sst>
 </file>
@@ -737,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -770,6 +785,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1096,17 +1117,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7A1970-D648-A84B-9973-6E2CBBFEC5E9}">
-  <dimension ref="A1:AH49"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -1114,7 +1135,7 @@
     <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="21" customWidth="1"/>
     <col min="12" max="15" width="6.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" customWidth="1"/>
     <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -1165,7 +1186,7 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="20" t="s">
         <v>14</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1259,7 +1280,7 @@
       <c r="J2" t="s">
         <v>38</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="21">
         <v>1094</v>
       </c>
       <c r="L2">
@@ -1320,7 +1341,7 @@
       <c r="J3" t="s">
         <v>42</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="21">
         <v>1392</v>
       </c>
       <c r="L3">
@@ -1366,7 +1387,7 @@
       <c r="J4" t="s">
         <v>46</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="21">
         <v>1386</v>
       </c>
       <c r="L4">
@@ -1412,7 +1433,7 @@
       <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="21">
         <v>1456</v>
       </c>
       <c r="L5">
@@ -1455,7 +1476,7 @@
       <c r="J6" t="s">
         <v>56</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="21">
         <v>1327</v>
       </c>
       <c r="L6">
@@ -1501,7 +1522,7 @@
       <c r="J7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="21">
         <v>1512</v>
       </c>
       <c r="L7">
@@ -1568,7 +1589,7 @@
       <c r="J8" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="22">
         <v>1316</v>
       </c>
       <c r="L8" s="10">
@@ -1635,7 +1656,7 @@
       <c r="J9" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="22">
         <v>1334</v>
       </c>
       <c r="L9" s="10">
@@ -1702,7 +1723,7 @@
       <c r="J10" t="s">
         <v>73</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="22">
         <v>1179</v>
       </c>
       <c r="L10" s="10">
@@ -1769,7 +1790,7 @@
       <c r="J11" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="22">
         <v>1348</v>
       </c>
       <c r="L11" s="10">
@@ -1814,7 +1835,7 @@
       <c r="J12" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="22">
         <v>1336</v>
       </c>
       <c r="L12" s="10">
@@ -1862,7 +1883,7 @@
       <c r="J13" t="s">
         <v>86</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="22">
         <v>1390</v>
       </c>
       <c r="L13" s="10">
@@ -1907,7 +1928,7 @@
       <c r="J14" t="s">
         <v>91</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="22">
         <v>1303</v>
       </c>
       <c r="L14" s="10">
@@ -1952,7 +1973,7 @@
       <c r="J15" t="s">
         <v>95</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="22">
         <v>1409</v>
       </c>
       <c r="L15" s="10">
@@ -1997,7 +2018,7 @@
       <c r="J16" t="s">
         <v>99</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="22">
         <v>1366</v>
       </c>
       <c r="L16" s="10">
@@ -2042,7 +2063,7 @@
       <c r="J17" t="s">
         <v>102</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="21">
         <v>1317</v>
       </c>
       <c r="L17">
@@ -2087,7 +2108,7 @@
       <c r="J18" t="s">
         <v>105</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="21">
         <v>1407</v>
       </c>
       <c r="L18">
@@ -2132,7 +2153,7 @@
       <c r="J19" t="s">
         <v>108</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="21">
         <v>1284</v>
       </c>
       <c r="L19">
@@ -2177,7 +2198,7 @@
       <c r="J20" t="s">
         <v>112</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="21">
         <v>1362</v>
       </c>
       <c r="L20">
@@ -2222,7 +2243,7 @@
       <c r="J21" t="s">
         <v>115</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="21">
         <v>1219</v>
       </c>
       <c r="L21">
@@ -2267,7 +2288,7 @@
       <c r="J22" t="s">
         <v>118</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="21">
         <v>1404</v>
       </c>
       <c r="L22">
@@ -2312,7 +2333,7 @@
       <c r="J23" t="s">
         <v>121</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="21">
         <v>1248</v>
       </c>
       <c r="L23">
@@ -2357,7 +2378,7 @@
       <c r="J24" t="s">
         <v>124</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="21">
         <v>1043</v>
       </c>
       <c r="L24">
@@ -2405,7 +2426,7 @@
       <c r="J25" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="23">
         <v>1090</v>
       </c>
       <c r="L25" s="14">
@@ -2453,7 +2474,7 @@
       <c r="J26" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="23">
         <v>1325</v>
       </c>
       <c r="L26" s="14">
@@ -2501,7 +2522,7 @@
       <c r="J27" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="K27" s="14">
+      <c r="K27" s="23">
         <v>1562</v>
       </c>
       <c r="L27" s="14">
@@ -2549,7 +2570,7 @@
       <c r="J28" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28" s="23">
         <v>1447</v>
       </c>
       <c r="L28" s="14">
@@ -2594,7 +2615,7 @@
       <c r="J29" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="23">
         <v>1245</v>
       </c>
       <c r="L29" s="14">
@@ -2639,7 +2660,7 @@
       <c r="J30" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="23">
         <v>1413</v>
       </c>
       <c r="L30" s="14">
@@ -2684,7 +2705,7 @@
       <c r="J31" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="K31" s="14">
+      <c r="K31" s="23">
         <v>1511</v>
       </c>
       <c r="L31" s="14">
@@ -2729,7 +2750,7 @@
       <c r="J32" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="K32" s="14">
+      <c r="K32" s="23">
         <v>1042</v>
       </c>
       <c r="L32" s="14">
@@ -2774,7 +2795,7 @@
       <c r="J33" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="21">
         <v>1188</v>
       </c>
       <c r="L33">
@@ -2819,7 +2840,7 @@
       <c r="J34" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="21">
         <v>1019</v>
       </c>
       <c r="L34">
@@ -2864,7 +2885,7 @@
       <c r="J35" t="s">
         <v>157</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="21">
         <v>1192</v>
       </c>
       <c r="L35">
@@ -2909,7 +2930,7 @@
       <c r="J36" t="s">
         <v>160</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="21">
         <v>1330</v>
       </c>
       <c r="L36">
@@ -2951,7 +2972,7 @@
       <c r="J37" t="s">
         <v>165</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="21">
         <v>414</v>
       </c>
       <c r="L37">
@@ -2996,7 +3017,7 @@
       <c r="J38" t="s">
         <v>171</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="21">
         <v>1343</v>
       </c>
       <c r="L38">
@@ -3041,7 +3062,7 @@
       <c r="J39" t="s">
         <v>175</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="21">
         <v>1005</v>
       </c>
       <c r="L39">
@@ -3085,7 +3106,7 @@
       <c r="J40" t="s">
         <v>181</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="21">
         <v>1425</v>
       </c>
       <c r="Q40" s="16" t="s">
@@ -3108,7 +3129,7 @@
       <c r="J41" t="s">
         <v>185</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="21">
         <v>1642</v>
       </c>
       <c r="Q41" s="16" t="s">
@@ -3131,7 +3152,7 @@
       <c r="J42" t="s">
         <v>189</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="21">
         <v>1749</v>
       </c>
       <c r="Q42" s="18" t="s">
@@ -3154,7 +3175,7 @@
       <c r="J43" t="s">
         <v>193</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="21">
         <v>1710</v>
       </c>
       <c r="Q43" s="18" t="s">
@@ -3177,7 +3198,7 @@
       <c r="J44" t="s">
         <v>196</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="21">
         <v>1548</v>
       </c>
       <c r="Q44" t="s">
@@ -3200,7 +3221,7 @@
       <c r="J45" t="s">
         <v>199</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="21">
         <v>1640</v>
       </c>
       <c r="Q45" t="s">
@@ -3223,7 +3244,7 @@
       <c r="J46" t="s">
         <v>202</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="21">
         <v>1715</v>
       </c>
       <c r="Q46" t="s">
@@ -3246,7 +3267,7 @@
       <c r="J47" t="s">
         <v>205</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="21">
         <v>1375</v>
       </c>
       <c r="Q47" t="s">
@@ -3269,7 +3290,7 @@
       <c r="J48" t="s">
         <v>209</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="21">
         <v>1424</v>
       </c>
       <c r="P48" s="18" t="s">
@@ -3279,7 +3300,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -3295,7 +3316,7 @@
       <c r="J49" t="s">
         <v>212</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="21">
         <v>1415</v>
       </c>
       <c r="P49" s="18" t="s">
@@ -3303,6 +3324,41 @@
       </c>
       <c r="Q49" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="18">
+        <v>43664</v>
+      </c>
+      <c r="J50" t="s">
+        <v>216</v>
+      </c>
+      <c r="K50" s="21">
+        <v>1498</v>
+      </c>
+      <c r="P50" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>217</v>
+      </c>
+      <c r="AE50">
+        <v>16.920000000000002</v>
+      </c>
+      <c r="AH50">
+        <v>1.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added coordinates excel sheets that are exported by crossROI
</commit_message>
<xml_diff>
--- a/mc4c_DatasetStatistics.xlsx
+++ b/mc4c_DatasetStatistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aallahyar/Technical/My_Works/MC-4C/67_MC4C_In_Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB876645-4986-944B-BE11-81F4553C8DE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A34F84-A2FD-C94F-8CAE-197945AD3178}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" xr2:uid="{F105A7CC-0618-604D-A8B3-8B950ADB213D}"/>
   </bookViews>
@@ -674,9 +674,6 @@
     <t>VER3768</t>
   </si>
   <si>
-    <t>nano cis</t>
-  </si>
-  <si>
     <t>refuel</t>
   </si>
   <si>
@@ -684,6 +681,9 @@
   </si>
   <si>
     <t>596ng</t>
+  </si>
+  <si>
+    <t>asMC4C_VP_B (Prdm14_RB_WT)</t>
   </si>
 </sst>
 </file>
@@ -1120,12 +1120,12 @@
   <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
     <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
@@ -3328,22 +3328,22 @@
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" t="s">
         <v>213</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>214</v>
       </c>
-      <c r="C50" t="s">
-        <v>215</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>1</v>
       </c>
       <c r="G50" s="18">
         <v>43664</v>
       </c>
       <c r="J50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K50" s="21">
         <v>1498</v>
@@ -3352,7 +3352,7 @@
         <v>162</v>
       </c>
       <c r="Q50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AE50">
         <v>16.920000000000002</v>

</xml_diff>